<commit_message>
Add readme, lookup table, and bookdown markdown files
</commit_message>
<xml_diff>
--- a/data/lookup/thresholding-lookup.xlsx
+++ b/data/lookup/thresholding-lookup.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\RegionalThresholds\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\RegionalThresholds\data\lookup\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA1E98BB-3AED-4750-92A3-2E3766C80AD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A89EC162-9BD4-4916-AB47-13B06DEF3A3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{4B537A8B-6999-40EC-B780-8F9E66433225}"/>
+    <workbookView xWindow="16380" yWindow="3420" windowWidth="14370" windowHeight="15840" xr2:uid="{4B537A8B-6999-40EC-B780-8F9E66433225}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -89,9 +89,6 @@
     <t>Wolverine</t>
   </si>
   <si>
-    <t>Threshold</t>
-  </si>
-  <si>
     <t>Taxon</t>
   </si>
   <si>
@@ -198,6 +195,9 @@
   </si>
   <si>
     <t>White-tailed Jack Rabbit</t>
+  </si>
+  <si>
+    <t>Threshold (%)</t>
   </si>
 </sst>
 </file>
@@ -552,7 +552,7 @@
   <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F32" sqref="F32"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -565,19 +565,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C1" t="s">
         <v>44</v>
       </c>
-      <c r="B1" t="s">
-        <v>46</v>
-      </c>
-      <c r="C1" t="s">
-        <v>45</v>
-      </c>
       <c r="D1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E1" t="s">
-        <v>17</v>
+        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -585,13 +585,13 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C2" t="s">
         <v>0</v>
       </c>
       <c r="D2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E2">
         <v>75</v>
@@ -599,16 +599,16 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B3" t="s">
         <v>48</v>
-      </c>
-      <c r="B3" t="s">
-        <v>49</v>
       </c>
       <c r="C3" t="s">
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E3">
         <v>50</v>
@@ -616,16 +616,16 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B4" t="s">
         <v>50</v>
-      </c>
-      <c r="B4" t="s">
-        <v>51</v>
       </c>
       <c r="C4" t="s">
         <v>2</v>
       </c>
       <c r="D4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E4">
         <v>50</v>
@@ -636,13 +636,13 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C5" t="s">
         <v>3</v>
       </c>
       <c r="D5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E5">
         <v>25</v>
@@ -653,13 +653,13 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
       </c>
       <c r="D6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E6">
         <v>25</v>
@@ -670,13 +670,13 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C7" t="s">
         <v>5</v>
       </c>
       <c r="D7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E7">
         <v>50</v>
@@ -687,13 +687,13 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C8" t="s">
         <v>6</v>
       </c>
       <c r="D8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E8">
         <v>75</v>
@@ -701,16 +701,16 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" t="s">
         <v>24</v>
-      </c>
-      <c r="B9" t="s">
-        <v>25</v>
       </c>
       <c r="C9" t="s">
         <v>7</v>
       </c>
       <c r="D9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E9">
         <v>25</v>
@@ -721,13 +721,13 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C10" t="s">
         <v>8</v>
       </c>
       <c r="D10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E10">
         <v>25</v>
@@ -738,13 +738,13 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C11" t="s">
         <v>9</v>
       </c>
       <c r="D11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E11">
         <v>25</v>
@@ -752,16 +752,16 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>27</v>
+      </c>
+      <c r="B12" t="s">
         <v>28</v>
-      </c>
-      <c r="B12" t="s">
-        <v>29</v>
       </c>
       <c r="C12" t="s">
         <v>10</v>
       </c>
       <c r="D12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E12">
         <v>75</v>
@@ -772,13 +772,13 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C13" t="s">
         <v>11</v>
       </c>
       <c r="D13" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E13">
         <v>100</v>
@@ -786,16 +786,16 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>30</v>
+      </c>
+      <c r="B14" t="s">
         <v>31</v>
-      </c>
-      <c r="B14" t="s">
-        <v>32</v>
       </c>
       <c r="C14" t="s">
         <v>12</v>
       </c>
       <c r="D14" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E14">
         <v>50</v>
@@ -803,16 +803,16 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>32</v>
+      </c>
+      <c r="B15" t="s">
         <v>33</v>
       </c>
-      <c r="B15" t="s">
-        <v>34</v>
-      </c>
       <c r="C15" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D15" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E15">
         <v>100</v>
@@ -820,16 +820,16 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>34</v>
+      </c>
+      <c r="B16" t="s">
         <v>35</v>
-      </c>
-      <c r="B16" t="s">
-        <v>36</v>
       </c>
       <c r="C16" t="s">
         <v>13</v>
       </c>
       <c r="D16" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E16">
         <v>50</v>
@@ -837,16 +837,16 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>36</v>
+      </c>
+      <c r="B17" t="s">
         <v>37</v>
-      </c>
-      <c r="B17" t="s">
-        <v>38</v>
       </c>
       <c r="C17" t="s">
         <v>15</v>
       </c>
       <c r="D17" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E17">
         <v>75</v>
@@ -854,16 +854,16 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>38</v>
+      </c>
+      <c r="B18" t="s">
         <v>39</v>
-      </c>
-      <c r="B18" t="s">
-        <v>40</v>
       </c>
       <c r="C18" t="s">
         <v>14</v>
       </c>
       <c r="D18" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E18">
         <v>25</v>
@@ -871,16 +871,16 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>40</v>
+      </c>
+      <c r="B19" t="s">
         <v>41</v>
       </c>
-      <c r="B19" t="s">
-        <v>42</v>
-      </c>
       <c r="C19" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D19" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E19">
         <v>100</v>
@@ -891,13 +891,13 @@
         <v>16</v>
       </c>
       <c r="B20" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C20" t="s">
         <v>16</v>
       </c>
       <c r="D20" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E20">
         <v>75</v>

</xml_diff>

<commit_message>
Adjust treshold for Wolverine and Grizzly Bear
</commit_message>
<xml_diff>
--- a/data/lookup/thresholding-lookup.xlsx
+++ b/data/lookup/thresholding-lookup.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\RegionalThresholds\data\lookup\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A89EC162-9BD4-4916-AB47-13B06DEF3A3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E1CBDC3-7E26-4C7D-845D-660D06A2C56D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16380" yWindow="3420" windowWidth="14370" windowHeight="15840" xr2:uid="{4B537A8B-6999-40EC-B780-8F9E66433225}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{4B537A8B-6999-40EC-B780-8F9E66433225}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="57">
   <si>
     <t>Badger</t>
   </si>
@@ -198,13 +198,22 @@
   </si>
   <si>
     <t>Threshold (%)</t>
+  </si>
+  <si>
+    <t>Grizzlybear</t>
+  </si>
+  <si>
+    <t>Ursus arctos</t>
+  </si>
+  <si>
+    <t>Grizzly Bear</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -212,16 +221,316 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -229,15 +538,205 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="42">
+    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -541,7 +1040,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -549,10 +1048,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7E8473A-43D2-4A78-9164-E21979B76636}">
-  <dimension ref="A1:E20"/>
+  <dimension ref="A1:V21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -563,7 +1062,7 @@
     <col min="4" max="4" width="26.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>43</v>
       </c>
@@ -580,7 +1079,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -597,7 +1096,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>47</v>
       </c>
@@ -614,7 +1113,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>49</v>
       </c>
@@ -631,7 +1130,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -648,7 +1147,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -665,7 +1164,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -682,7 +1181,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -699,7 +1198,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>23</v>
       </c>
@@ -716,32 +1215,48 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E10" s="1">
+        <v>75</v>
+      </c>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+      <c r="K10" s="1"/>
+      <c r="L10" s="1"/>
+      <c r="M10" s="1"/>
+      <c r="N10" s="1"/>
+      <c r="O10" s="1"/>
+      <c r="P10" s="1"/>
+      <c r="Q10" s="1"/>
+      <c r="R10" s="1"/>
+      <c r="S10" s="1"/>
+      <c r="T10" s="1"/>
+      <c r="U10" s="1"/>
+      <c r="V10" s="1"/>
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>8</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B11" t="s">
         <v>25</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C11" t="s">
         <v>8</v>
-      </c>
-      <c r="D10" t="s">
-        <v>18</v>
-      </c>
-      <c r="E10">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>9</v>
-      </c>
-      <c r="B11" t="s">
-        <v>26</v>
-      </c>
-      <c r="C11" t="s">
-        <v>9</v>
       </c>
       <c r="D11" t="s">
         <v>18</v>
@@ -750,157 +1265,174 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12" t="s">
+        <v>9</v>
+      </c>
+      <c r="D12" t="s">
+        <v>18</v>
+      </c>
+      <c r="E12">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>27</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B13" t="s">
         <v>28</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C13" t="s">
         <v>10</v>
       </c>
-      <c r="D12" t="s">
-        <v>18</v>
-      </c>
-      <c r="E12">
+      <c r="D13" t="s">
+        <v>18</v>
+      </c>
+      <c r="E13">
         <v>75</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>11</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B14" t="s">
         <v>29</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C14" t="s">
         <v>11</v>
       </c>
-      <c r="D13" t="s">
-        <v>18</v>
-      </c>
-      <c r="E13">
+      <c r="D14" t="s">
+        <v>18</v>
+      </c>
+      <c r="E14">
         <v>100</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>30</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B15" t="s">
         <v>31</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C15" t="s">
         <v>12</v>
       </c>
-      <c r="D14" t="s">
-        <v>18</v>
-      </c>
-      <c r="E14">
+      <c r="D15" t="s">
+        <v>18</v>
+      </c>
+      <c r="E15">
         <v>50</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>32</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B16" t="s">
         <v>33</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C16" t="s">
         <v>51</v>
       </c>
-      <c r="D15" t="s">
-        <v>18</v>
-      </c>
-      <c r="E15">
+      <c r="D16" t="s">
+        <v>18</v>
+      </c>
+      <c r="E16">
         <v>100</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>34</v>
-      </c>
-      <c r="B16" t="s">
-        <v>35</v>
-      </c>
-      <c r="C16" t="s">
-        <v>13</v>
-      </c>
-      <c r="D16" t="s">
-        <v>18</v>
-      </c>
-      <c r="E16">
-        <v>50</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B17" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C17" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D17" t="s">
         <v>18</v>
       </c>
       <c r="E17">
-        <v>75</v>
+        <v>50</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B18" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C18" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D18" t="s">
         <v>18</v>
       </c>
       <c r="E18">
-        <v>25</v>
+        <v>75</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B19" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C19" t="s">
-        <v>52</v>
+        <v>14</v>
       </c>
       <c r="D19" t="s">
         <v>18</v>
       </c>
       <c r="E19">
-        <v>100</v>
+        <v>25</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
+        <v>40</v>
+      </c>
+      <c r="B20" t="s">
+        <v>41</v>
+      </c>
+      <c r="C20" t="s">
+        <v>52</v>
+      </c>
+      <c r="D20" t="s">
+        <v>18</v>
+      </c>
+      <c r="E20">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
         <v>16</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B21" t="s">
         <v>42</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C21" t="s">
         <v>16</v>
       </c>
-      <c r="D20" t="s">
-        <v>18</v>
-      </c>
-      <c r="E20">
-        <v>75</v>
+      <c r="D21" t="s">
+        <v>18</v>
+      </c>
+      <c r="E21">
+        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>